<commit_message>
Minor fixes to various chapters
Minor fixes were made to several chapters.
</commit_message>
<xml_diff>
--- a/DHS7tabplan/Tab_Plan_Chap04_Marriage_and_Sexual_Activity_VII_13April2018.xlsx
+++ b/DHS7tabplan/Tab_Plan_Chap04_Marriage_and_Sexual_Activity_VII_13April2018.xlsx
@@ -6547,8 +6547,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A3299ADD5D91FC4981A62029954D61DA" ma:contentTypeVersion="476" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="95dfcc87ed256f4aed73fd9ca228c514">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd" xmlns:ns3="d16efad5-0601-4cf0-b7c2-89968258c777" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="88209df52733b038c0f2ab805b0d468e" ns1:_="" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A3299ADD5D91FC4981A62029954D61DA" ma:contentTypeVersion="481" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="be21cae339529f0f311ef097f4a87693">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd" xmlns:ns3="d16efad5-0601-4cf0-b7c2-89968258c777" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fd9e5a0c56088652e9b5d1a36fcd7f8a" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd"/>
     <xsd:import namespace="d16efad5-0601-4cf0-b7c2-89968258c777"/>
@@ -6572,6 +6572,10 @@
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns2:Survey_x0020_Type" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -6634,6 +6638,28 @@
           <xsd:enumeration value="DHS"/>
           <xsd:enumeration value="MIS"/>
           <xsd:enumeration value="SPA"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="23" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="24" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="25" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="26" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
@@ -6864,7 +6890,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE0C9E42-E7D2-4D40-B51E-4D86B212BDA2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85992D2E-5675-4CE4-8869-16F0149235CD}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>